<commit_message>
update form ver 2
</commit_message>
<xml_diff>
--- a/Kichban/kichban_normal_after6.xlsx
+++ b/Kichban/kichban_normal_after6.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Kịch bản</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Max_Số khoảng cách ngày muốn dự đoán trong tương lai (k)</t>
   </si>
   <si>
-    <t>Thuộc tính biết trong t+k ngày</t>
-  </si>
-  <si>
     <t>Thuộc tính biết trong t ngày</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
   </si>
   <si>
     <t>Ngưỡng sai số dự đoán cho phép</t>
-  </si>
-  <si>
-    <t>Chuẩn hóa dữ liệu</t>
   </si>
   <si>
     <t>SMOTE</t>
@@ -90,8 +84,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
@@ -126,6 +120,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -134,13 +135,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -151,22 +145,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -181,7 +160,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -203,6 +197,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -211,6 +212,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -219,8 +227,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,21 +237,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -257,25 +251,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,138 +419,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -426,18 +432,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,11 +447,18 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,15 +474,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,9 +504,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,33 +542,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -569,130 +563,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1020,10 +1014,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -1032,13 +1026,12 @@
     <col min="2" max="2" width="63.9047619047619" customWidth="1"/>
     <col min="3" max="3" width="40.7238095238095" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="7" max="7" width="45.2666666666667" customWidth="1"/>
-    <col min="8" max="8" width="71.5428571428571" customWidth="1"/>
-    <col min="9" max="9" width="22.5428571428571" customWidth="1"/>
-    <col min="15" max="15" width="10.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="71.5428571428571" customWidth="1"/>
+    <col min="8" max="8" width="22.5428571428571" customWidth="1"/>
+    <col min="13" max="13" width="10.2857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="135" spans="1:15">
+    <row r="1" ht="135" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1072,31 +1065,25 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -1104,40 +1091,40 @@
       <c r="F2">
         <v>6</v>
       </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
       <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="I2">
+        <v>14</v>
       </c>
       <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>1.2</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="N2">
         <v>100</v>
       </c>
-      <c r="O2">
+      <c r="M2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>6</v>
@@ -1145,25 +1132,25 @@
       <c r="F3">
         <v>6</v>
       </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
       <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="I3">
+        <v>14</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>1.2</v>
       </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
       <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="N3">
         <v>100</v>
       </c>
-      <c r="O3">
+      <c r="M3">
         <v>30</v>
       </c>
     </row>

</xml_diff>